<commit_message>
protected sheets and minor instruction changes
</commit_message>
<xml_diff>
--- a/RosterValidationErrorTool.xlsx
+++ b/RosterValidationErrorTool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\userFiles\andrew.cornish\Documents\nwE\GitHub\Roster_Validation_Error_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDBCA7E-1D21-491E-AFBE-E5B7BAB39CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B300DB9-2CBC-4070-82D6-22A539C927FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="4" xr2:uid="{985D94C2-37CC-4D82-BC01-A17C2CF3E421}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" xr2:uid="{985D94C2-37CC-4D82-BC01-A17C2CF3E421}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="278">
   <si>
     <t>Note: orange highlight = manual/set var</t>
   </si>
@@ -1180,42 +1180,6 @@
   </si>
   <si>
     <t>inc/decr tool?? - 1 to Count(errors) .. Can't do both (this and Col B of errors)..  Causes security warning due to tool</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>ow4270302</t>
-  </si>
-  <si>
-    <t>or874256648</t>
-  </si>
-  <si>
-    <t>or792138279</t>
-  </si>
-  <si>
-    <t>or447968054</t>
-  </si>
-  <si>
-    <t>bartholomeow.quinn@nwea.pottsboro.com</t>
-  </si>
-  <si>
-    <t>2012/25/5</t>
-  </si>
-  <si>
-    <t>ow4270303</t>
-  </si>
-  <si>
-    <t>or065773275</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>ow4270304</t>
-  </si>
-  <si>
-    <t>ff</t>
   </si>
   <si>
     <t xml:space="preserve">Possible? </t>
@@ -2751,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E8B01C-6CD5-4B10-98F2-4E6C450A9BE0}">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,7 +2762,7 @@
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="str">
         <f ca="1">IFERROR(IF(Calcs!B14=0,helpText!A5,Calcs!B21),"")</f>
-        <v>Roster file does not appear to be open</v>
+        <v/>
       </c>
       <c r="C5" s="101"/>
       <c r="D5" s="102"/>
@@ -2820,7 +2784,7 @@
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="97" t="str">
         <f ca="1">"Erroneuous Data : "&amp;IF(Calcs!B20=Calcs!X9,TEXT(Calcs!B29,"mm/dd/yyyy"),Calcs!B29)</f>
-        <v>Erroneuous Data : ow4270302</v>
+        <v xml:space="preserve">Erroneuous Data : </v>
       </c>
       <c r="C8" s="98"/>
       <c r="D8" s="99"/>
@@ -2837,15 +2801,15 @@
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="73" t="str">
         <f ca="1">"Heading : "&amp;IFERROR(Calcs!B20,"")</f>
-        <v>Heading : Instructor ID</v>
-      </c>
-      <c r="C10" s="76" t="e">
+        <v>Heading : 0</v>
+      </c>
+      <c r="C10" s="76" t="str">
         <f ca="1">Calcs!D20</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D10" s="74">
+        <v/>
+      </c>
+      <c r="D10" s="74" t="str">
         <f ca="1">Calcs!D21</f>
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -2859,7 +2823,7 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="106" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">IFERROR(INDIRECT("helpText!"&amp;ADDRESS(MATCH(TRUE,EXACT(B5,helpText!A2:A30),0)+1,2,4)),"No additional help found")</f>
-        <v>Ensure 'trngact2.csv' is also open.</v>
+        <v>Error is a blank row or not recognized</v>
       </c>
       <c r="C12" s="107"/>
       <c r="D12" s="108"/>
@@ -2877,15 +2841,15 @@
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="117" t="e">
         <f ca="1">IF(OR(Calcs!$B$72=1,AND(Calcs!$B$22=1, LEN(Calcs!F21)&gt;0),AND(NOT(Calcs!$B$29=Calcs!$F$21),Calcs!$B$72=0)),"May have been corrected by previous change","")</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="C15" s="118"/>
       <c r="D15" s="119"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="120" t="e">
+      <c r="B16" s="120" t="str">
         <f ca="1">IF(Calcs!B15,IF(AND(Calcs!D22,NOT(Calcs!F22)),"ERRONEOUOS DATA MISSING - see instructions",""),"LAST ROW ERROR - see instuctions sheet")</f>
-        <v>#REF!</v>
+        <v>LAST ROW ERROR - see instuctions sheet</v>
       </c>
       <c r="C16" s="120"/>
       <c r="D16" s="120"/>
@@ -3196,7 +3160,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,23 +3207,13 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="str">
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
-        <v>Current</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E3" s="47">
-        <v>2</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>177</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="51"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3267,21 +3221,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E4" s="47">
-        <v>2</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>178</v>
-      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="51"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3289,21 +3233,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B5" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="47">
-        <v>2</v>
-      </c>
-      <c r="F5" s="47" t="s">
-        <v>179</v>
-      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="51"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3311,21 +3245,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B6" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E6" s="47">
-        <v>2</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>180</v>
-      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3333,21 +3257,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>277</v>
-      </c>
-      <c r="E7" s="47">
-        <v>3</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>128</v>
-      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="51"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3355,21 +3269,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B8" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="E8" s="47">
-        <v>7</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>181</v>
-      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3377,21 +3281,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B9" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>279</v>
-      </c>
-      <c r="E9" s="47">
-        <v>10</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>128</v>
-      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
       <c r="G9" s="51"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3399,21 +3293,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B10" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>279</v>
-      </c>
-      <c r="E10" s="47">
-        <v>10</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>182</v>
-      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3421,21 +3305,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B11" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="E11" s="47">
-        <v>11</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>95</v>
-      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="51"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3443,21 +3317,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B12" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="E12" s="47">
-        <v>11</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>94</v>
-      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
       <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3465,21 +3329,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B13" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="E13" s="47">
-        <v>12</v>
-      </c>
-      <c r="F13" s="47" t="s">
-        <v>102</v>
-      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
       <c r="G13" s="51"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3487,21 +3341,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="E14" s="47">
-        <v>12</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>129</v>
-      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
       <c r="G14" s="51"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3509,21 +3353,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B15" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>283</v>
-      </c>
-      <c r="E15" s="47">
-        <v>18</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>183</v>
-      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
       <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3531,21 +3365,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B16" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>284</v>
-      </c>
-      <c r="E16" s="47">
-        <v>18</v>
-      </c>
-      <c r="F16" s="47" t="s">
-        <v>131</v>
-      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
       <c r="G16" s="51"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3553,21 +3377,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B17" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="E17" s="47">
-        <v>20</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>179</v>
-      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
       <c r="G17" s="51"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3575,21 +3389,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B18" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>286</v>
-      </c>
-      <c r="E18" s="47">
-        <v>27</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>131</v>
-      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
       <c r="G18" s="51"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3597,21 +3401,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B19" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="47">
-        <v>189945</v>
-      </c>
-      <c r="E19" s="47">
-        <v>29</v>
-      </c>
-      <c r="F19" s="47" t="s">
-        <v>178</v>
-      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="51"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3619,19 +3413,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B20" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>27</v>
-      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="47"/>
-      <c r="E20" s="47">
-        <v>33</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="51"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3639,19 +3425,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B21" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>43</v>
-      </c>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="47"/>
-      <c r="E21" s="47">
-        <v>34</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
       <c r="G21" s="51"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3659,19 +3437,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B22" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>30</v>
-      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="47"/>
-      <c r="E22" s="47">
-        <v>34</v>
-      </c>
-      <c r="F22" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
       <c r="G22" s="51"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3679,19 +3449,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B23" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>184</v>
-      </c>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="47"/>
-      <c r="E23" s="47">
-        <v>34</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
       <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3699,19 +3461,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B24" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>37</v>
-      </c>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="47"/>
-      <c r="E24" s="47">
-        <v>35</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
       <c r="G24" s="49"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3719,19 +3473,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B25" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>42</v>
-      </c>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
       <c r="D25" s="47"/>
-      <c r="E25" s="47">
-        <v>35</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
       <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3739,19 +3485,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B26" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>185</v>
-      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
       <c r="D26" s="47"/>
-      <c r="E26" s="47">
-        <v>35</v>
-      </c>
-      <c r="F26" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
       <c r="G26" s="49"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3759,19 +3497,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B27" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>41</v>
-      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
       <c r="D27" s="47"/>
-      <c r="E27" s="47">
-        <v>36</v>
-      </c>
-      <c r="F27" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
       <c r="G27" s="49"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3779,19 +3509,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B28" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>20</v>
-      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
       <c r="D28" s="47"/>
-      <c r="E28" s="47">
-        <v>36</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
       <c r="G28" s="49"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3799,19 +3521,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B29" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="47"/>
-      <c r="E29" s="47">
-        <v>36</v>
-      </c>
-      <c r="F29" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
       <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3819,19 +3533,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B30" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>130</v>
-      </c>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
       <c r="D30" s="47"/>
-      <c r="E30" s="47">
-        <v>37</v>
-      </c>
-      <c r="F30" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="49"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3839,19 +3545,11 @@
         <f ca="1">IFERROR(IF(ROW()=Calcs!$B$19,Calcs!$D$5,""),"")</f>
         <v/>
       </c>
-      <c r="B31" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>18</v>
-      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="47"/>
-      <c r="E31" s="47">
-        <v>37</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>93</v>
-      </c>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="49"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4188,7 +3886,7 @@
   <dimension ref="A1:AC86"/>
   <sheetViews>
     <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="J90" sqref="J90"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4466,121 +4164,121 @@
       <c r="AC10" s="9"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="e" cm="1">
+      <c r="A11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(A9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B11" s="6" t="e" cm="1">
+        <v>P</v>
+      </c>
+      <c r="B11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="B11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(B9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C11" s="6" t="e" cm="1">
+        <v>A</v>
+      </c>
+      <c r="C11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(C9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D11" s="6" t="e" cm="1">
+        <v>Q</v>
+      </c>
+      <c r="D11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(D9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E11" s="6" t="e" cm="1">
+        <v>B</v>
+      </c>
+      <c r="E11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(E9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F11" s="6" t="e" cm="1">
+        <v>R</v>
+      </c>
+      <c r="F11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(F9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G11" s="6" t="e" cm="1">
+        <v>C</v>
+      </c>
+      <c r="G11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(G9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H11" s="6" t="e" cm="1">
+        <v>D</v>
+      </c>
+      <c r="H11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(H9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I11" s="6" t="e" cm="1">
+        <v>S</v>
+      </c>
+      <c r="I11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(I9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="6" t="e" cm="1">
+        <v>E</v>
+      </c>
+      <c r="J11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(J9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K11" s="6" t="e" cm="1">
+        <v>F</v>
+      </c>
+      <c r="K11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(K9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L11" s="6" t="e" cm="1">
+        <v>G</v>
+      </c>
+      <c r="L11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(L9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M11" s="6" t="e" cm="1">
+        <v>T</v>
+      </c>
+      <c r="M11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="M11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(M9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N11" s="6" t="e" cm="1">
+        <v>U</v>
+      </c>
+      <c r="N11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="N11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(N9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O11" s="6" t="e" cm="1">
+        <v>H</v>
+      </c>
+      <c r="O11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(O9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P11" s="6" t="e" cm="1">
+        <v>V</v>
+      </c>
+      <c r="P11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="P11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(P9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q11" s="6" t="e" cm="1">
+        <v>W</v>
+      </c>
+      <c r="Q11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(Q9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R11" s="6" t="e" cm="1">
+        <v>X</v>
+      </c>
+      <c r="R11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="R11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(R9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S11" s="6" t="e" cm="1">
+        <v>Y</v>
+      </c>
+      <c r="S11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(S9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T11" s="6" t="e" cm="1">
+        <v>Z</v>
+      </c>
+      <c r="T11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(T9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U11" s="6" t="e" cm="1">
+        <v>AA</v>
+      </c>
+      <c r="U11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(U9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V11" s="6" t="e" cm="1">
+        <v>I</v>
+      </c>
+      <c r="V11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(V9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W11" s="6" t="e" cm="1">
+        <v>J</v>
+      </c>
+      <c r="W11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(W9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X11" s="6" t="e" cm="1">
+        <v>AB</v>
+      </c>
+      <c r="X11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(X9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Y11" s="6" t="e" cm="1">
+        <v>K</v>
+      </c>
+      <c r="Y11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(Y9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Z11" s="6" t="e" cm="1">
+        <v>L</v>
+      </c>
+      <c r="Z11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="Z11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(Z9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AA11" s="6" t="e" cm="1">
+        <v>M</v>
+      </c>
+      <c r="AA11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="AA11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(AA9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AB11" s="6" t="e" cm="1">
+        <v>N</v>
+      </c>
+      <c r="AB11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="AB11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(AB9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AC11" s="6" t="e" cm="1">
+        <v>O</v>
+      </c>
+      <c r="AC11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="AC11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(AC9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>#REF!</v>
+        <v>AC</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -4589,16 +4287,16 @@
       </c>
       <c r="B14" s="22" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">IFERROR(MAX(IF(ISBLANK(INDIRECT($B$7&amp;$B$11&amp;":"&amp;$B$11)),0,ROW(INDIRECT($B$7&amp;$B$11&amp;":"&amp;$B$11)))),0)</f>
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="22" t="e" cm="1">
+      <c r="B15" s="22" t="b" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">SUMPRODUCT(--(INDIRECT(B7&amp;J5&amp;B14+1&amp;":"&amp;K5&amp;B14+101)&lt;&gt;""))=0</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4610,7 +4308,7 @@
       </c>
       <c r="G17" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">RIGHT(TRIM(INDIRECT(B2&amp;"$"&amp;E4&amp;"$"&amp;B19)),LEN(B5))</f>
-        <v>is ID</v>
+        <v/>
       </c>
       <c r="H17" s="6" t="b">
         <f ca="1">G17=B5</f>
@@ -4632,23 +4330,23 @@
       </c>
       <c r="B19" s="22" cm="1">
         <f t="array" aca="1" ref="B19" ca="1">_xlfn.IFNA(ROW(INDEX(INDIRECT(B18),MATCH(TRUE,INDEX((INDIRECT(B18)&lt;&gt;0),0),0))),99)</f>
-        <v>3</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="B20" s="21" t="str" cm="1">
+      <c r="B20" s="21" cm="1">
         <f t="array" aca="1" ref="B20" ca="1">IF(ISBLANK(INDIRECT(B2&amp;"$"&amp;B4&amp;"$"&amp;B19)),0,INDIRECT(B2&amp;"$"&amp;B4&amp;"$"&amp;B19))</f>
-        <v>Instructor ID</v>
+        <v>0</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="24" t="e" cm="1">
+      <c r="D20" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">IFERROR(IF(B20&lt;&gt;0,INDIRECT(ADDRESS(ROW(A11),MATCH(B20,A9:AC9,0),4)),""),INDIRECT(ADDRESS(ROW(A27),MATCH(B20,A26:H26,0),4)))</f>
-        <v>#N/A</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4657,25 +4355,25 @@
       </c>
       <c r="B21" s="26" t="str" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">IF(B20&lt;&gt;0,TRIM(INDIRECT(B2&amp;"$"&amp;E4&amp;"$"&amp;B19)),"")</f>
-        <v>First Name must be the same for this ID</v>
+        <v/>
       </c>
       <c r="C21" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="26" cm="1">
+      <c r="D21" s="26" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">IF(B20&lt;&gt;0,INDIRECT(B2&amp;D4&amp;B19),"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E21" s="17" t="s">
         <v>97</v>
       </c>
       <c r="F21" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">IF(AND(B22,ISBLANK(INDIRECT(B7&amp;D20&amp;D21))),"",INDIRECT(B7&amp;D20&amp;D21))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="G21" s="22" t="e">
         <f ca="1">LEN(F21)</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4691,7 +4389,7 @@
       </c>
       <c r="D22" s="21" t="b" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">ISBLANK(INDIRECT(B2&amp;"$"&amp;C4&amp;"$"&amp;B19))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>269</v>
@@ -4735,13 +4433,13 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="e">
+      <c r="A27" s="12" t="str">
         <f ca="1">G11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B27" s="12" t="e">
+        <v>D</v>
+      </c>
+      <c r="B27" s="12" t="str">
         <f ca="1">F11</f>
-        <v>#REF!</v>
+        <v>C</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -4756,7 +4454,7 @@
       </c>
       <c r="B29" s="22" t="str" cm="1">
         <f t="array" aca="1" ref="B29" ca="1">IF(ISBLANK(INDIRECT(B2&amp;C4&amp;B19)),"",INDIRECT(B2&amp;C4&amp;B19))</f>
-        <v>ow4270302</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4781,11 +4479,11 @@
       </c>
       <c r="B33" s="6" t="b">
         <f ca="1">ISNUMBER(SEARCH(B32,B21))</f>
-        <v>1</v>
-      </c>
-      <c r="C33" s="6" t="str">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6" t="e">
         <f ca="1">MID(B21,FIND("@",SUBSTITUTE(B21," ","@",LEN(B21)-LEN(SUBSTITUTE(B21," ",""))-1))+1,100)</f>
-        <v>this ID</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4794,7 +4492,7 @@
       </c>
       <c r="B37" s="22" cm="1">
         <f t="array" aca="1" ref="B37" ca="1">IF(NOT(B22),IFERROR(IFERROR(SEARCH(B32,INDIRECT($B$2&amp;"$"&amp;$E$4&amp;"$"&amp;$B$19)),SEARCH(C32,INDIRECT($B$2&amp;"$"&amp;$E$4&amp;"$"&amp;$B$19))),0),0)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>55</v>
@@ -4809,7 +4507,7 @@
       </c>
       <c r="B38" s="21">
         <f ca="1">IF(AND(B22=0,B37&gt;0),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -4818,7 +4516,7 @@
       </c>
       <c r="B39" s="22" t="str">
         <f ca="1">IF(B38,TRIM(LEFT(B21,B37-1)),"")</f>
-        <v>First Name</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -4832,22 +4530,22 @@
       <c r="A42" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="22" t="str">
+      <c r="B42" s="22" t="e">
         <f ca="1">IF(NOT($B$33),MID(B21,FIND("@",SUBSTITUTE(B21," ","@",LEN(B21)-LEN(SUBSTITUTE(B21," ",""))-1))+1,100),"")</f>
-        <v/>
-      </c>
-      <c r="E42" s="6" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E42" s="6" t="e">
         <f ca="1">IF(B33,B20,B42)</f>
-        <v>Instructor ID</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="21">
+      <c r="B43" s="21" t="e">
         <f ca="1">IF(AND(NOT(B33),OR(B42=D9,B42=N9)),1,0)</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -4863,7 +4561,7 @@
       </c>
       <c r="B47" s="22">
         <f ca="1">IF(OR(B20=D9,B20=N9),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>61</v>
@@ -4882,9 +4580,9 @@
       <c r="A49" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="21" t="str">
+      <c r="B49" s="21" t="e">
         <f ca="1">IF(B33,B20,B42)</f>
-        <v>Instructor ID</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>148</v>
@@ -4908,25 +4606,25 @@
       <c r="A52" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="21" t="str">
+      <c r="B52" s="21" t="e">
         <f ca="1">IF(OR(AND(B47,B33),AND(B43,NOT(B33))),LEFT(B49,(FIND(" ",B49,1)-1)),0)</f>
-        <v>Instructor</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E52" s="6" t="str">
+      <c r="E52" s="6" t="e">
         <f ca="1">IF(OR(AND(B47,B33),AND(B43,NOT(B33))),LEFT(B49,(FIND(" ",B49,1)-1)),IF(AND(NOT(B47),B33),"this is true",0))</f>
-        <v>Instructor</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="22" t="str">
+      <c r="B53" s="22" t="e">
         <f ca="1">B52&amp;" "&amp;B39</f>
-        <v>Instructor First Name</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G53" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="G53" ca="1">INDIRECT(ADDRESS(ROW(A57),MATCH(TRUE,EXACT(B49,A56:G56),0),4))</f>
@@ -5056,9 +4754,9 @@
       <c r="A62" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="22" t="str" cm="1">
+      <c r="B62" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="B62" ca="1">IFERROR(INDIRECT(ADDRESS(ROW(A60),MATCH(TRUE,EXACT(B53,A59:AC59),0),4)),B53)</f>
-        <v>Instructor First Name</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.25">
@@ -5076,9 +4774,9 @@
       <c r="A65" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B65" s="22" t="str">
+      <c r="B65" s="22" t="e">
         <f ca="1">IF(B33,B62,B42)</f>
-        <v>Instructor First Name</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>157</v>
@@ -5090,7 +4788,7 @@
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H66" s="6" t="str">
         <f ca="1">$B$7&amp;"$"&amp;$B$67&amp;"$2:$"&amp;$B$67&amp;"$"&amp;B14&amp;"----"&amp;$B$7&amp;"$"&amp;$B$67&amp;"$2:$"&amp;$B$67&amp;"$"&amp;B14</f>
-        <v>'trngact2.csv'!$error$2:$error$0----'trngact2.csv'!$error$2:$error$0</v>
+        <v>'trngact2.csv'!$error$2:$error$36----'trngact2.csv'!$error$2:$error$36</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5121,7 +4819,7 @@
       </c>
       <c r="B69" s="22" t="str">
         <f ca="1">$B$7&amp;"$"&amp;$B$67&amp;"$2:$"&amp;$B$67&amp;"$"&amp;B14</f>
-        <v>'trngact2.csv'!$error$2:$error$0</v>
+        <v>'trngact2.csv'!$error$2:$error$36</v>
       </c>
       <c r="E69" s="29" t="s">
         <v>88</v>
@@ -5134,9 +4832,9 @@
       <c r="A70" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="21" t="e">
+      <c r="B70" s="21" t="str">
         <f ca="1">$B$7&amp;"$"&amp;$D$20&amp;"$2:$"&amp;$D$20&amp;"$"&amp;B14</f>
-        <v>#N/A</v>
+        <v>'trngact2.csv'!$$2:$$36</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5417,8 +5115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECFE470-B3BD-410D-AC44-F3675458F186}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5577,7 +5275,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="71" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5709,8 +5407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D84B839-E1BE-4EE3-B57B-7F90F98A7800}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5893,7 +5591,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -5901,7 +5599,7 @@
         <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -6080,6 +5778,7 @@
     <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="AHYkEWQitLWW96cXkZ+/2CrRan4CJNLBubNiLibb2uc9Np9+2WdBGsk1w/Wz98gMHcYs02WkHicuUDQJcAghTQ==" saltValue="frUOipYUIcLnQ601tZ4SJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="A44:B44"/>
@@ -6106,7 +5805,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6285,6 +5984,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="IzfhpOKm2QFC+l0sTzoP6l1I5vvGbiXBXWBYVmKNvG6UybRCuJYLqkq50Trnclsm55GkGaa8akhoL+Xx7hHUUA==" saltValue="POJhJOzOCN1QUt8D9y169A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changed fileNames and updated Readme
</commit_message>
<xml_diff>
--- a/RosterValidationErrorTool.xlsx
+++ b/RosterValidationErrorTool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\userFiles\andrew.cornish\Documents\nwE\GitHub\Roster_Validation_Error_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B300DB9-2CBC-4070-82D6-22A539C927FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E944F683-0DD2-490C-94D8-35D84B04CF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" xr2:uid="{985D94C2-37CC-4D82-BC01-A17C2CF3E421}"/>
   </bookViews>
@@ -1176,9 +1176,6 @@
     <t xml:space="preserve">  This file is only for assisting with finding the 'format errors' that were detected during an import.  It does not detect errors on its own, instead it utilizes the errors copied from the associated 'Export - File Validation Errors.cvs' to display helpful information concerning each particular error.</t>
   </si>
   <si>
-    <t>trngact2</t>
-  </si>
-  <si>
     <t>inc/decr tool?? - 1 to Count(errors) .. Can't do both (this and Col B of errors)..  Causes security warning due to tool</t>
   </si>
   <si>
@@ -1189,6 +1186,9 @@
   </si>
   <si>
     <t>Only the top most error (with 'RF') will be used by the tool.</t>
+  </si>
+  <si>
+    <t>exRoster</t>
   </si>
 </sst>
 </file>
@@ -2172,6 +2172,36 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2189,36 +2219,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2716,7 +2716,7 @@
   <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="90" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C2" s="91"/>
       <c r="D2" s="92"/>
@@ -2762,7 +2762,7 @@
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="str">
         <f ca="1">IFERROR(IF(Calcs!B14=0,helpText!A5,Calcs!B21),"")</f>
-        <v/>
+        <v>Roster file does not appear to be open</v>
       </c>
       <c r="C5" s="101"/>
       <c r="D5" s="102"/>
@@ -2823,7 +2823,7 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="106" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">IFERROR(INDIRECT("helpText!"&amp;ADDRESS(MATCH(TRUE,EXACT(B5,helpText!A2:A30),0)+1,2,4)),"No additional help found")</f>
-        <v>Error is a blank row or not recognized</v>
+        <v>Ensure 'exRoster.csv' is also open.</v>
       </c>
       <c r="C12" s="107"/>
       <c r="D12" s="108"/>
@@ -2847,9 +2847,9 @@
       <c r="D15" s="119"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="120" t="str">
+      <c r="B16" s="120" t="e">
         <f ca="1">IF(Calcs!B15,IF(AND(Calcs!D22,NOT(Calcs!F22)),"ERRONEOUOS DATA MISSING - see instructions",""),"LAST ROW ERROR - see instuctions sheet")</f>
-        <v>LAST ROW ERROR - see instuctions sheet</v>
+        <v>#REF!</v>
       </c>
       <c r="C16" s="120"/>
       <c r="D16" s="120"/>
@@ -3904,7 +3904,7 @@
       </c>
       <c r="B1" s="22" t="str">
         <f>Dashboard!B2&amp;".csv"</f>
-        <v>trngact2.csv</v>
+        <v>exRoster.csv</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>0</v>
@@ -4030,11 +4030,11 @@
       </c>
       <c r="B7" s="17" t="str">
         <f>"'"&amp;Calcs!B1&amp;"'!"</f>
-        <v>'trngact2.csv'!</v>
+        <v>'exRoster.csv'!</v>
       </c>
       <c r="C7" s="17" t="str">
         <f>B7&amp;J5&amp;L5&amp;":"&amp;K5&amp;L5</f>
-        <v>'trngact2.csv'!$A$1:$AC$1</v>
+        <v>'exRoster.csv'!$A$1:$AC$1</v>
       </c>
       <c r="F7" s="17"/>
     </row>
@@ -4164,121 +4164,121 @@
       <c r="AC10" s="9"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="str" cm="1">
+      <c r="A11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(A9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>P</v>
-      </c>
-      <c r="B11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="B11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="B11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(B9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>A</v>
-      </c>
-      <c r="C11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="C11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(C9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>Q</v>
-      </c>
-      <c r="D11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="D11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(D9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>B</v>
-      </c>
-      <c r="E11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(E9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>R</v>
-      </c>
-      <c r="F11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="F11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(F9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>C</v>
-      </c>
-      <c r="G11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="G11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(G9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>D</v>
-      </c>
-      <c r="H11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="H11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(H9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>S</v>
-      </c>
-      <c r="I11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="I11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(I9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>E</v>
-      </c>
-      <c r="J11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="J11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(J9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>F</v>
-      </c>
-      <c r="K11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(K9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>G</v>
-      </c>
-      <c r="L11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="L11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(L9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>T</v>
-      </c>
-      <c r="M11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="M11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="M11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(M9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>U</v>
-      </c>
-      <c r="N11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="N11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="N11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(N9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>H</v>
-      </c>
-      <c r="O11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="O11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(O9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>V</v>
-      </c>
-      <c r="P11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="P11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="P11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(P9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>W</v>
-      </c>
-      <c r="Q11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="Q11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(Q9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>X</v>
-      </c>
-      <c r="R11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="R11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="R11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(R9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>Y</v>
-      </c>
-      <c r="S11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="S11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(S9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>Z</v>
-      </c>
-      <c r="T11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="T11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(T9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>AA</v>
-      </c>
-      <c r="U11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="U11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(U9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>I</v>
-      </c>
-      <c r="V11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="V11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(V9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>J</v>
-      </c>
-      <c r="W11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="W11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(W9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>AB</v>
-      </c>
-      <c r="X11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="X11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(X9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>K</v>
-      </c>
-      <c r="Y11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="Y11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(Y9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>L</v>
-      </c>
-      <c r="Z11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="Z11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="Z11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(Z9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>M</v>
-      </c>
-      <c r="AA11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="AA11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="AA11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(AA9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>N</v>
-      </c>
-      <c r="AB11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="AB11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="AB11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(AB9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>O</v>
-      </c>
-      <c r="AC11" s="6" t="str" cm="1">
+        <v>#REF!</v>
+      </c>
+      <c r="AC11" s="6" t="e" cm="1">
         <f t="array" aca="1" ref="AC11" ca="1">SUBSTITUTE(ADDRESS(1,MATCH(TRUE,EXACT(AC9,INDIRECT($C$7)),0),4),1,"")</f>
-        <v>AC</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -4287,16 +4287,16 @@
       </c>
       <c r="B14" s="22" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">IFERROR(MAX(IF(ISBLANK(INDIRECT($B$7&amp;$B$11&amp;":"&amp;$B$11)),0,ROW(INDIRECT($B$7&amp;$B$11&amp;":"&amp;$B$11)))),0)</f>
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="22" t="b" cm="1">
+      <c r="B15" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">SUMPRODUCT(--(INDIRECT(B7&amp;J5&amp;B14+1&amp;":"&amp;K5&amp;B14+101)&lt;&gt;""))=0</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4433,13 +4433,13 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="str">
+      <c r="A27" s="12" t="e">
         <f ca="1">G11</f>
-        <v>D</v>
-      </c>
-      <c r="B27" s="12" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="B27" s="12" t="e">
         <f ca="1">F11</f>
-        <v>C</v>
+        <v>#REF!</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -4788,7 +4788,7 @@
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H66" s="6" t="str">
         <f ca="1">$B$7&amp;"$"&amp;$B$67&amp;"$2:$"&amp;$B$67&amp;"$"&amp;B14&amp;"----"&amp;$B$7&amp;"$"&amp;$B$67&amp;"$2:$"&amp;$B$67&amp;"$"&amp;B14</f>
-        <v>'trngact2.csv'!$error$2:$error$36----'trngact2.csv'!$error$2:$error$36</v>
+        <v>'exRoster.csv'!$error$2:$error$0----'exRoster.csv'!$error$2:$error$0</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B69" s="22" t="str">
         <f ca="1">$B$7&amp;"$"&amp;$B$67&amp;"$2:$"&amp;$B$67&amp;"$"&amp;B14</f>
-        <v>'trngact2.csv'!$error$2:$error$36</v>
+        <v>'exRoster.csv'!$error$2:$error$0</v>
       </c>
       <c r="E69" s="29" t="s">
         <v>88</v>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="B70" s="21" t="str">
         <f ca="1">$B$7&amp;"$"&amp;$D$20&amp;"$2:$"&amp;$D$20&amp;"$"&amp;B14</f>
-        <v>'trngact2.csv'!$$2:$$36</v>
+        <v>'exRoster.csv'!$$2:$$0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5270,12 +5270,12 @@
         <v>227</v>
       </c>
       <c r="C27" s="71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="71" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5435,20 +5435,20 @@
       <c r="A3" s="50">
         <v>1</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="126" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="133"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="127"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
@@ -5478,17 +5478,17 @@
       <c r="A10" s="50">
         <v>2</v>
       </c>
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="126" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="126"/>
       <c r="M10" s="49"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -5591,7 +5591,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -5599,7 +5599,7 @@
         <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -5608,165 +5608,165 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="131" t="s">
+      <c r="A36" s="141" t="s">
         <v>272</v>
       </c>
-      <c r="B36" s="131"/>
-      <c r="C36" s="131"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="131"/>
-      <c r="F36" s="131"/>
-      <c r="G36" s="131"/>
-      <c r="H36" s="131"/>
-      <c r="I36" s="131"/>
-      <c r="J36" s="131"/>
-      <c r="K36" s="131"/>
-      <c r="L36" s="131"/>
-      <c r="M36" s="131"/>
+      <c r="B36" s="141"/>
+      <c r="C36" s="141"/>
+      <c r="D36" s="141"/>
+      <c r="E36" s="141"/>
+      <c r="F36" s="141"/>
+      <c r="G36" s="141"/>
+      <c r="H36" s="141"/>
+      <c r="I36" s="141"/>
+      <c r="J36" s="141"/>
+      <c r="K36" s="141"/>
+      <c r="L36" s="141"/>
+      <c r="M36" s="141"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="131"/>
-      <c r="B37" s="131"/>
-      <c r="C37" s="131"/>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="131"/>
-      <c r="H37" s="131"/>
-      <c r="I37" s="131"/>
-      <c r="J37" s="131"/>
-      <c r="K37" s="131"/>
-      <c r="L37" s="131"/>
-      <c r="M37" s="131"/>
+      <c r="A37" s="141"/>
+      <c r="B37" s="141"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="141"/>
+      <c r="E37" s="141"/>
+      <c r="F37" s="141"/>
+      <c r="G37" s="141"/>
+      <c r="H37" s="141"/>
+      <c r="I37" s="141"/>
+      <c r="J37" s="141"/>
+      <c r="K37" s="141"/>
+      <c r="L37" s="141"/>
+      <c r="M37" s="141"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
-      <c r="B38" s="131"/>
-      <c r="C38" s="131"/>
-      <c r="D38" s="131"/>
-      <c r="E38" s="131"/>
-      <c r="F38" s="131"/>
-      <c r="G38" s="131"/>
-      <c r="H38" s="131"/>
-      <c r="I38" s="131"/>
-      <c r="J38" s="131"/>
-      <c r="K38" s="131"/>
-      <c r="L38" s="131"/>
-      <c r="M38" s="131"/>
+      <c r="A38" s="141"/>
+      <c r="B38" s="141"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="141"/>
+      <c r="G38" s="141"/>
+      <c r="H38" s="141"/>
+      <c r="I38" s="141"/>
+      <c r="J38" s="141"/>
+      <c r="K38" s="141"/>
+      <c r="L38" s="141"/>
+      <c r="M38" s="141"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="131"/>
-      <c r="B39" s="131"/>
-      <c r="C39" s="131"/>
-      <c r="D39" s="131"/>
-      <c r="E39" s="131"/>
-      <c r="F39" s="131"/>
-      <c r="G39" s="131"/>
-      <c r="H39" s="131"/>
-      <c r="I39" s="131"/>
-      <c r="J39" s="131"/>
-      <c r="K39" s="131"/>
-      <c r="L39" s="131"/>
-      <c r="M39" s="131"/>
+      <c r="A39" s="141"/>
+      <c r="B39" s="141"/>
+      <c r="C39" s="141"/>
+      <c r="D39" s="141"/>
+      <c r="E39" s="141"/>
+      <c r="F39" s="141"/>
+      <c r="G39" s="141"/>
+      <c r="H39" s="141"/>
+      <c r="I39" s="141"/>
+      <c r="J39" s="141"/>
+      <c r="K39" s="141"/>
+      <c r="L39" s="141"/>
+      <c r="M39" s="141"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
-      <c r="B40" s="131"/>
-      <c r="C40" s="131"/>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="131"/>
-      <c r="H40" s="131"/>
-      <c r="I40" s="131"/>
-      <c r="J40" s="131"/>
-      <c r="K40" s="131"/>
-      <c r="L40" s="131"/>
-      <c r="M40" s="131"/>
+      <c r="A40" s="141"/>
+      <c r="B40" s="141"/>
+      <c r="C40" s="141"/>
+      <c r="D40" s="141"/>
+      <c r="E40" s="141"/>
+      <c r="F40" s="141"/>
+      <c r="G40" s="141"/>
+      <c r="H40" s="141"/>
+      <c r="I40" s="141"/>
+      <c r="J40" s="141"/>
+      <c r="K40" s="141"/>
+      <c r="L40" s="141"/>
+      <c r="M40" s="141"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="136" t="s">
+      <c r="A43" s="130" t="s">
         <v>250</v>
       </c>
-      <c r="B43" s="136"/>
-      <c r="C43" s="136"/>
-      <c r="D43" s="136"/>
-      <c r="E43" s="136"/>
-      <c r="F43" s="136"/>
-      <c r="G43" s="136"/>
-      <c r="H43" s="136"/>
-      <c r="I43" s="136"/>
-      <c r="J43" s="136"/>
-      <c r="K43" s="136"/>
-      <c r="L43" s="136"/>
-      <c r="M43" s="136"/>
-      <c r="N43" s="136"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="130"/>
+      <c r="D43" s="130"/>
+      <c r="E43" s="130"/>
+      <c r="F43" s="130"/>
+      <c r="G43" s="130"/>
+      <c r="H43" s="130"/>
+      <c r="I43" s="130"/>
+      <c r="J43" s="130"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="130"/>
+      <c r="M43" s="130"/>
+      <c r="N43" s="130"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="134" t="s">
+      <c r="A44" s="128" t="s">
         <v>251</v>
       </c>
-      <c r="B44" s="135"/>
-      <c r="C44" s="139" t="s">
+      <c r="B44" s="129"/>
+      <c r="C44" s="133" t="s">
         <v>253</v>
       </c>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140" t="s">
+      <c r="D44" s="134"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="134"/>
+      <c r="G44" s="134"/>
+      <c r="H44" s="134"/>
+      <c r="I44" s="134" t="s">
         <v>254</v>
       </c>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="140"/>
-      <c r="M44" s="140"/>
-      <c r="N44" s="140"/>
+      <c r="J44" s="134"/>
+      <c r="K44" s="134"/>
+      <c r="L44" s="134"/>
+      <c r="M44" s="134"/>
+      <c r="N44" s="134"/>
     </row>
     <row r="45" spans="1:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="137" t="s">
+      <c r="A45" s="131" t="s">
         <v>252</v>
       </c>
-      <c r="B45" s="137"/>
-      <c r="C45" s="138" t="s">
+      <c r="B45" s="131"/>
+      <c r="C45" s="132" t="s">
         <v>265</v>
       </c>
-      <c r="D45" s="138"/>
-      <c r="E45" s="138"/>
-      <c r="F45" s="138"/>
-      <c r="G45" s="138"/>
-      <c r="H45" s="138"/>
-      <c r="I45" s="141" t="s">
+      <c r="D45" s="132"/>
+      <c r="E45" s="132"/>
+      <c r="F45" s="132"/>
+      <c r="G45" s="132"/>
+      <c r="H45" s="132"/>
+      <c r="I45" s="135" t="s">
         <v>255</v>
       </c>
-      <c r="J45" s="141"/>
-      <c r="K45" s="141"/>
-      <c r="L45" s="141"/>
-      <c r="M45" s="141"/>
-      <c r="N45" s="141"/>
+      <c r="J45" s="135"/>
+      <c r="K45" s="135"/>
+      <c r="L45" s="135"/>
+      <c r="M45" s="135"/>
+      <c r="N45" s="135"/>
     </row>
     <row r="46" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="126" t="s">
+      <c r="A46" s="136" t="s">
         <v>263</v>
       </c>
-      <c r="B46" s="126"/>
-      <c r="C46" s="127" t="s">
+      <c r="B46" s="136"/>
+      <c r="C46" s="137" t="s">
         <v>264</v>
       </c>
-      <c r="D46" s="128"/>
-      <c r="E46" s="128"/>
-      <c r="F46" s="128"/>
-      <c r="G46" s="128"/>
-      <c r="H46" s="128"/>
-      <c r="I46" s="129" t="s">
+      <c r="D46" s="138"/>
+      <c r="E46" s="138"/>
+      <c r="F46" s="138"/>
+      <c r="G46" s="138"/>
+      <c r="H46" s="138"/>
+      <c r="I46" s="139" t="s">
         <v>266</v>
       </c>
-      <c r="J46" s="130"/>
-      <c r="K46" s="130"/>
-      <c r="L46" s="130"/>
-      <c r="M46" s="130"/>
-      <c r="N46" s="130"/>
+      <c r="J46" s="140"/>
+      <c r="K46" s="140"/>
+      <c r="L46" s="140"/>
+      <c r="M46" s="140"/>
+      <c r="N46" s="140"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="71"/>
@@ -5780,6 +5780,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="AHYkEWQitLWW96cXkZ+/2CrRan4CJNLBubNiLibb2uc9Np9+2WdBGsk1w/Wz98gMHcYs02WkHicuUDQJcAghTQ==" saltValue="frUOipYUIcLnQ601tZ4SJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="A36:M40"/>
+    <mergeCell ref="B10:J10"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A43:N43"/>
@@ -5788,11 +5793,6 @@
     <mergeCell ref="C44:H44"/>
     <mergeCell ref="I44:N44"/>
     <mergeCell ref="I45:N45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="A36:M40"/>
-    <mergeCell ref="B10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="B5" s="79" t="str">
         <f>"Ensure '"&amp;Calcs!B1&amp;"' is also open."</f>
-        <v>Ensure 'trngact2.csv' is also open.</v>
+        <v>Ensure 'exRoster.csv' is also open.</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>